<commit_message>
New file for text function
</commit_message>
<xml_diff>
--- a/Text_functions.xlsx
+++ b/Text_functions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data-Analyst9\Excel\Practice\dateFunction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4023D48-7D4A-40C7-98C6-3767C2BB7C78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16D7405B-E3DC-49CD-BB6F-16B820EC2B13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>ShopName</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>zudio</t>
+  </si>
+  <si>
+    <t>Sr No</t>
   </si>
 </sst>
 </file>
@@ -390,15 +393,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="E7:O12"/>
+  <dimension ref="D7:O12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="7" spans="5:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
       <c r="E7" t="s">
         <v>0</v>
       </c>
@@ -433,7 +439,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="5:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D8">
+        <v>1</v>
+      </c>
       <c r="E8" t="s">
         <v>11</v>
       </c>
@@ -468,7 +477,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="5:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D9">
+        <v>2</v>
+      </c>
       <c r="E9" t="s">
         <v>12</v>
       </c>
@@ -503,7 +515,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="5:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D10">
+        <v>3</v>
+      </c>
       <c r="E10" t="s">
         <v>13</v>
       </c>
@@ -538,7 +553,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="5:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D11">
+        <v>4</v>
+      </c>
       <c r="E11" t="s">
         <v>14</v>
       </c>
@@ -573,7 +591,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="5:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D12">
+        <v>5</v>
+      </c>
       <c r="E12" t="s">
         <v>15</v>
       </c>

</xml_diff>